<commit_message>
Parse data from google sheets
</commit_message>
<xml_diff>
--- a/newsletters/db/emails.xlsx
+++ b/newsletters/db/emails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>shyue@example.com</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>ruby-tips</t>
+  </si>
+  <si>
+    <t>vim-tips</t>
+  </si>
+  <si>
+    <t>python-tips</t>
+  </si>
+  <si>
+    <t>scott</t>
+  </si>
+  <si>
+    <t>scott@scott.com</t>
+  </si>
+  <si>
+    <t>alice</t>
+  </si>
+  <si>
+    <t>alice@example.com</t>
+  </si>
+  <si>
+    <t>no-tips</t>
   </si>
 </sst>
 </file>
@@ -64,9 +91,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,7 +101,7 @@
     <font>
       <u/>
       <sz val="12"/>
-      <color theme="10"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,16 +124,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -437,55 +468,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -494,8 +563,11 @@
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>